<commit_message>
I changed all of the graphs to bar graphs and completed the first draft of the Board Snapshot
</commit_message>
<xml_diff>
--- a/experiments/Combined A-D.xlsx
+++ b/experiments/Combined A-D.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6440" yWindow="0" windowWidth="30360" windowHeight="20260" tabRatio="500" activeTab="6"/>
+    <workbookView xWindow="2220" yWindow="0" windowWidth="29480" windowHeight="19880" tabRatio="500" firstSheet="1" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="A1" sheetId="3" r:id="rId1"/>
@@ -197,8 +197,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="39">
+  <cellStyleXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -250,7 +262,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="39">
+  <cellStyles count="51">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -270,6 +282,12 @@
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -289,6 +307,12 @@
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -456,11 +480,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="424303272"/>
-        <c:axId val="424310168"/>
+        <c:axId val="392497720"/>
+        <c:axId val="392504616"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="424303272"/>
+        <c:axId val="392497720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -488,7 +512,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="424310168"/>
+        <c:crossAx val="392504616"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -496,7 +520,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="424310168"/>
+        <c:axId val="392504616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -526,7 +550,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="424303272"/>
+        <c:crossAx val="392497720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -708,11 +732,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="422964584"/>
-        <c:axId val="422970344"/>
+        <c:axId val="392588632"/>
+        <c:axId val="392594392"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="422964584"/>
+        <c:axId val="392588632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -745,7 +769,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="422970344"/>
+        <c:crossAx val="392594392"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -753,7 +777,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="422970344"/>
+        <c:axId val="392594392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -783,7 +807,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="422964584"/>
+        <c:crossAx val="392588632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -965,11 +989,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="423018056"/>
-        <c:axId val="423023816"/>
+        <c:axId val="392641624"/>
+        <c:axId val="392647384"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="423018056"/>
+        <c:axId val="392641624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1002,7 +1026,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="423023816"/>
+        <c:crossAx val="392647384"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1010,7 +1034,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="423023816"/>
+        <c:axId val="392647384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1045,7 +1069,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="423018056"/>
+        <c:crossAx val="392641624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1230,11 +1254,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="424373064"/>
-        <c:axId val="424378616"/>
+        <c:axId val="392693944"/>
+        <c:axId val="392699464"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="424373064"/>
+        <c:axId val="392693944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1262,7 +1286,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="424378616"/>
+        <c:crossAx val="392699464"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1270,7 +1294,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="424378616"/>
+        <c:axId val="392699464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1300,7 +1324,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="424373064"/>
+        <c:crossAx val="392693944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1336,11 +1360,31 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="4000"/>
+              <a:t>Distance at 0 Feet With Rotation</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -1348,14 +1392,12 @@
           <c:tx>
             <c:v>A1</c:v>
           </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'A1'!$A$2:$A$8</c:f>
+              <c:f>'D2'!$A$2:$A$9</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>0ft</c:v>
                 </c:pt>
@@ -1376,6 +1418,9 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>30ft</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>35ft</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1410,7 +1455,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -1418,14 +1462,12 @@
           <c:tx>
             <c:v>A2</c:v>
           </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'A1'!$A$2:$A$8</c:f>
+              <c:f>'D2'!$A$2:$A$9</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>0ft</c:v>
                 </c:pt>
@@ -1446,6 +1488,9 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>30ft</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>35ft</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1480,7 +1525,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -1488,9 +1532,39 @@
           <c:tx>
             <c:v>B1</c:v>
           </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'D2'!$A$2:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0ft</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5ft</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10ft</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15ft</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20ft</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25ft</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>30ft</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>35ft</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>'B1'!$I$2:$I$8</c:f>
@@ -1521,7 +1595,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -1529,9 +1602,39 @@
           <c:tx>
             <c:v>B2</c:v>
           </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'D2'!$A$2:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0ft</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5ft</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10ft</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15ft</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20ft</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25ft</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>30ft</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>35ft</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>'B2'!$I$2:$I$8</c:f>
@@ -1562,7 +1665,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="4"/>
@@ -1570,9 +1672,39 @@
           <c:tx>
             <c:v>C1</c:v>
           </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'D2'!$A$2:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0ft</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5ft</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10ft</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15ft</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20ft</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25ft</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>30ft</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>35ft</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>'C1'!$I$2:$I$8</c:f>
@@ -1603,7 +1735,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="5"/>
@@ -1611,9 +1742,39 @@
           <c:tx>
             <c:v>C2</c:v>
           </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'D2'!$A$2:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0ft</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5ft</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10ft</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15ft</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20ft</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25ft</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>30ft</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>35ft</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>'C2'!$I$2:$I$8</c:f>
@@ -1644,7 +1805,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="6"/>
@@ -1652,9 +1812,39 @@
           <c:tx>
             <c:v>D1</c:v>
           </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'D2'!$A$2:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0ft</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5ft</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10ft</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15ft</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20ft</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25ft</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>30ft</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>35ft</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>'D1'!$I$2:$I$8</c:f>
@@ -1685,7 +1875,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="7"/>
@@ -1693,9 +1882,39 @@
           <c:tx>
             <c:v>D2</c:v>
           </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'D2'!$A$2:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0ft</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5ft</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10ft</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15ft</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20ft</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25ft</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>30ft</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>35ft</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>'D2'!$I$2:$I$9</c:f>
@@ -1729,7 +1948,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1739,22 +1957,50 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="424435256"/>
-        <c:axId val="424438232"/>
-      </c:lineChart>
+        <c:gapWidth val="150"/>
+        <c:axId val="392763128"/>
+        <c:axId val="392766104"/>
+      </c:barChart>
       <c:catAx>
-        <c:axId val="424435256"/>
+        <c:axId val="392763128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="2800"/>
+                  <a:t>Distance (feet)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="424438232"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="392766104"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1762,18 +2008,47 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="424438232"/>
+        <c:axId val="392766104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="2800"/>
+                  <a:t>Times seen per second</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="424435256"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="392763128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1782,6 +2057,16 @@
       <c:legendPos val="r"/>
       <c:layout/>
       <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600"/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
@@ -1809,6 +2094,25 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="4000"/>
+              <a:t>Relative Rotation Graph</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -1820,8 +2124,16 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>A1-B1</c:v>
+            <c:v>B1-A1</c:v>
           </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="tx2">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
@@ -1862,22 +2174,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.0321149122967483</c:v>
+                  <c:v>-0.0321149122967483</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>21.42167595168938</c:v>
+                  <c:v>-21.42167595168938</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-6.769204203608621</c:v>
+                  <c:v>6.769204203608621</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.779342242439048</c:v>
+                  <c:v>-0.779342242439048</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.5</c:v>
+                  <c:v>-0.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.2</c:v>
+                  <c:v>-0.2</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0.0</c:v>
@@ -1890,8 +2202,16 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>A1-B2</c:v>
+            <c:v>B2-A1</c:v>
           </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="tx2">
+                <a:lumMod val="40000"/>
+                <a:lumOff val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
@@ -1932,22 +2252,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1.399485366657799</c:v>
+                  <c:v>-1.399485366657799</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>23.82158631568369</c:v>
+                  <c:v>-23.82158631568369</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-4.211556965746817</c:v>
+                  <c:v>4.211556965746817</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.779342242439048</c:v>
+                  <c:v>-0.779342242439048</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.5</c:v>
+                  <c:v>-0.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.2</c:v>
+                  <c:v>-0.2</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0.0</c:v>
@@ -1960,8 +2280,15 @@
           <c:idx val="2"/>
           <c:order val="2"/>
           <c:tx>
-            <c:v>A1-C1</c:v>
+            <c:v>C1-A1</c:v>
           </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:lumMod val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
@@ -2002,22 +2329,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.474955867996329</c:v>
+                  <c:v>-0.474955867996329</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>26.86040265373215</c:v>
+                  <c:v>-26.86040265373215</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.4</c:v>
+                  <c:v>-6.4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-3.975892831720401</c:v>
+                  <c:v>3.975892831720401</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-1.388530913495015</c:v>
+                  <c:v>1.388530913495015</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.2</c:v>
+                  <c:v>-0.2</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0.0</c:v>
@@ -2030,8 +2357,16 @@
           <c:idx val="3"/>
           <c:order val="3"/>
           <c:tx>
-            <c:v>A1-C2</c:v>
+            <c:v>C2-A1</c:v>
           </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
@@ -2072,25 +2407,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.709180885607189</c:v>
+                  <c:v>-0.709180885607189</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10.60237758903902</c:v>
+                  <c:v>-10.60237758903902</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.000000000000001</c:v>
+                  <c:v>-5.000000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-3.51597060873814</c:v>
+                  <c:v>3.51597060873814</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-0.5</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>-0.1</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>0.1</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>-0.1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2100,8 +2435,15 @@
           <c:idx val="4"/>
           <c:order val="4"/>
           <c:tx>
-            <c:v>A1-D1</c:v>
+            <c:v>D1-A1</c:v>
           </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4">
+                <a:lumMod val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
@@ -2142,25 +2484,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.722049570423408</c:v>
+                  <c:v>-0.722049570423408</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18.72702205401377</c:v>
+                  <c:v>-18.72702205401377</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.369316581882128</c:v>
+                  <c:v>0.369316581882128</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.679342242439048</c:v>
+                  <c:v>-0.679342242439048</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.6</c:v>
+                  <c:v>-0.6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-0.2</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-0.2</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2170,8 +2512,16 @@
           <c:idx val="5"/>
           <c:order val="5"/>
           <c:tx>
-            <c:v>A1-D2</c:v>
+            <c:v>D2-A1</c:v>
           </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
@@ -2212,28 +2562,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1.8471457615275</c:v>
+                  <c:v>-1.8471457615275</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.47786233194973</c:v>
+                  <c:v>-4.47786233194973</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-4.560898654163157</c:v>
+                  <c:v>4.560898654163157</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-7.793947982980073</c:v>
+                  <c:v>7.793947982980073</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-3.0</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-2.3</c:v>
+                  <c:v>2.3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-0.2</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-0.8</c:v>
+                  <c:v>0.8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2248,20 +2598,49 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="424478200"/>
-        <c:axId val="424481256"/>
+        <c:axId val="392812536"/>
+        <c:axId val="392815672"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="424478200"/>
+        <c:axId val="392812536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="2800"/>
+                  <a:t>Distance (feet)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="424481256"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="392815672"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2269,18 +2648,47 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="424481256"/>
+        <c:axId val="392815672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="2800"/>
+                  <a:t>Number of more times seen per second</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="424478200"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="392812536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2289,6 +2697,16 @@
       <c:legendPos val="r"/>
       <c:layout/>
       <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600"/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
@@ -3090,7 +3508,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="S28" sqref="S28"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData/>
@@ -3383,7 +3803,7 @@
   <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3458,8 +3878,8 @@
         <v>55.362081701868725</v>
       </c>
       <c r="K2">
-        <f>'A1'!I2-'B1'!I2</f>
-        <v>3.2114912296748344E-2</v>
+        <f>'B1'!I2-'A1'!I2</f>
+        <v>-3.2114912296748344E-2</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -3493,8 +3913,8 @@
         <v>17.403330276330248</v>
       </c>
       <c r="K3">
-        <f>'A1'!I3-'B1'!I3</f>
-        <v>21.421675951689384</v>
+        <f>'B1'!I3-'A1'!I3</f>
+        <v>-21.421675951689384</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -3528,8 +3948,8 @@
         <v>15.069204203608622</v>
       </c>
       <c r="K4">
-        <f>'A1'!I4-'B1'!I4</f>
-        <v>-6.7692042036086217</v>
+        <f>'B1'!I4-'A1'!I4</f>
+        <v>6.7692042036086217</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -3541,8 +3961,8 @@
         <v>0</v>
       </c>
       <c r="K5">
-        <f>'A1'!I5-'B1'!I5</f>
-        <v>0.77934224243904837</v>
+        <f>'B1'!I5-'A1'!I5</f>
+        <v>-0.77934224243904837</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -3576,8 +3996,8 @@
         <v>0.1</v>
       </c>
       <c r="K6">
-        <f>'A1'!I6-'B1'!I6</f>
-        <v>0.5</v>
+        <f>'B1'!I6-'A1'!I6</f>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -3588,8 +4008,8 @@
         <v>0</v>
       </c>
       <c r="K7">
-        <f>'A1'!I7-'B1'!I7</f>
-        <v>0.2</v>
+        <f>'B1'!I7-'A1'!I7</f>
+        <v>-0.2</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -3600,7 +4020,7 @@
         <v>0</v>
       </c>
       <c r="K8">
-        <f>'A1'!I8-'B1'!I8</f>
+        <f>'B1'!I8-'A1'!I8</f>
         <v>0</v>
       </c>
     </row>
@@ -3621,7 +4041,7 @@
   <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection sqref="A1:I1"/>
+      <selection activeCell="K3" sqref="K3:K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3695,8 +4115,8 @@
         <v>53.994711247507674</v>
       </c>
       <c r="K2">
-        <f>'A1'!I2-'B2'!I2</f>
-        <v>1.3994853666577995</v>
+        <f>'B2'!I2-'A1'!I2</f>
+        <v>-1.3994853666577995</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -3730,8 +4150,8 @@
         <v>15.003419912335946</v>
       </c>
       <c r="K3">
-        <f>'A1'!I3-'B2'!I3</f>
-        <v>23.821586315683685</v>
+        <f>'B2'!I3-'A1'!I3</f>
+        <v>-23.821586315683685</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -3765,8 +4185,8 @@
         <v>12.511556965746818</v>
       </c>
       <c r="K4">
-        <f>'A1'!I4-'B2'!I4</f>
-        <v>-4.2115569657468175</v>
+        <f>'B2'!I4-'A1'!I4</f>
+        <v>4.2115569657468175</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -3777,8 +4197,8 @@
         <v>0</v>
       </c>
       <c r="K5">
-        <f>'A1'!I5-'B2'!I5</f>
-        <v>0.77934224243904837</v>
+        <f>'B2'!I5-'A1'!I5</f>
+        <v>-0.77934224243904837</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -3812,8 +4232,8 @@
         <v>0.1</v>
       </c>
       <c r="K6">
-        <f>'A1'!I6-'B2'!I6</f>
-        <v>0.5</v>
+        <f>'B2'!I6-'A1'!I6</f>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -3824,8 +4244,8 @@
         <v>0</v>
       </c>
       <c r="K7">
-        <f>'A1'!I7-'B2'!I7</f>
-        <v>0.2</v>
+        <f>'B2'!I7-'A1'!I7</f>
+        <v>-0.2</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -3836,7 +4256,7 @@
         <v>0</v>
       </c>
       <c r="K8">
-        <f>'A1'!I8-'B2'!I8</f>
+        <f>'B2'!I8-'A1'!I8</f>
         <v>0</v>
       </c>
     </row>
@@ -3856,7 +4276,7 @@
   <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3931,8 +4351,8 @@
         <v>54.919240746169145</v>
       </c>
       <c r="K2">
-        <f>'A1'!I2-'C1'!I2</f>
-        <v>0.47495586799632861</v>
+        <f>'C1'!I2-'A1'!I2</f>
+        <v>-0.47495586799632861</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -3966,8 +4386,8 @@
         <v>11.96460357428748</v>
       </c>
       <c r="K3">
-        <f>'A1'!I3-'C1'!I3</f>
-        <v>26.860402653732152</v>
+        <f>'C1'!I3-'A1'!I3</f>
+        <v>-26.860402653732152</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -4001,8 +4421,8 @@
         <v>1.9</v>
       </c>
       <c r="K4">
-        <f>'A1'!I4-'C1'!I4</f>
-        <v>6.4</v>
+        <f>'C1'!I4-'A1'!I4</f>
+        <v>-6.4</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -4036,8 +4456,8 @@
         <v>4.7552350741594491</v>
       </c>
       <c r="K5">
-        <f>'A1'!I5-'C1'!I5</f>
-        <v>-3.975892831720401</v>
+        <f>'C1'!I5-'A1'!I5</f>
+        <v>3.975892831720401</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -4071,8 +4491,8 @@
         <v>1.9885309134950155</v>
       </c>
       <c r="K6">
-        <f>'A1'!I6-'C1'!I6</f>
-        <v>-1.3885309134950155</v>
+        <f>'C1'!I6-'A1'!I6</f>
+        <v>1.3885309134950155</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -4083,8 +4503,8 @@
         <v>0</v>
       </c>
       <c r="K7">
-        <f>'A1'!I7-'C1'!I7</f>
-        <v>0.2</v>
+        <f>'C1'!I7-'A1'!I7</f>
+        <v>-0.2</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -4095,7 +4515,7 @@
         <v>0</v>
       </c>
       <c r="K8">
-        <f>'A1'!I8-'C1'!I8</f>
+        <f>'C1'!I8-'A1'!I8</f>
         <v>0</v>
       </c>
     </row>
@@ -4116,7 +4536,7 @@
   <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection sqref="A1:I1"/>
+      <selection activeCell="K3" sqref="K3:K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4191,8 +4611,8 @@
         <v>54.685015728558284</v>
       </c>
       <c r="K2">
-        <f>'A1'!I2-'C2'!I2</f>
-        <v>0.70918088560718928</v>
+        <f>'C2'!I2-'A1'!I2</f>
+        <v>-0.70918088560718928</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -4226,8 +4646,8 @@
         <v>28.222628638980616</v>
       </c>
       <c r="K3">
-        <f>'A1'!I3-'C2'!I3</f>
-        <v>10.602377589039016</v>
+        <f>'C2'!I3-'A1'!I3</f>
+        <v>-10.602377589039016</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -4261,8 +4681,8 @@
         <v>3.3</v>
       </c>
       <c r="K4">
-        <f>'A1'!I4-'C2'!I4</f>
-        <v>5.0000000000000009</v>
+        <f>'C2'!I4-'A1'!I4</f>
+        <v>-5.0000000000000009</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -4296,8 +4716,8 @@
         <v>4.2953128511771883</v>
       </c>
       <c r="K5">
-        <f>'A1'!I5-'C2'!I5</f>
-        <v>-3.5159706087381402</v>
+        <f>'C2'!I5-'A1'!I5</f>
+        <v>3.5159706087381402</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -4331,8 +4751,8 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="K6">
-        <f>'A1'!I6-'C2'!I6</f>
-        <v>-0.50000000000000011</v>
+        <f>'C2'!I6-'A1'!I6</f>
+        <v>0.50000000000000011</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -4366,8 +4786,8 @@
         <v>0.1</v>
       </c>
       <c r="K7">
-        <f>'A1'!I7-'C2'!I7</f>
-        <v>0.1</v>
+        <f>'C2'!I7-'A1'!I7</f>
+        <v>-0.1</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -4401,8 +4821,8 @@
         <v>0.1</v>
       </c>
       <c r="K8">
-        <f>'A1'!I8-'C2'!I8</f>
-        <v>-0.1</v>
+        <f>'C2'!I8-'A1'!I8</f>
+        <v>0.1</v>
       </c>
     </row>
   </sheetData>
@@ -4420,8 +4840,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3:K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4495,8 +4915,8 @@
         <v>54.672147043742065</v>
       </c>
       <c r="K2">
-        <f>'A1'!I2-'D1'!I2</f>
-        <v>0.72204957042340823</v>
+        <f>'D1'!I2-'A1'!I2</f>
+        <v>-0.72204957042340823</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -4530,8 +4950,8 @@
         <v>20.097984174005866</v>
       </c>
       <c r="K3">
-        <f>'A1'!I3-'D1'!I3</f>
-        <v>18.727022054013766</v>
+        <f>'D1'!I3-'A1'!I3</f>
+        <v>-18.727022054013766</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -4565,8 +4985,8 @@
         <v>8.6693165818821285</v>
       </c>
       <c r="K4">
-        <f>'A1'!I4-'D1'!I4</f>
-        <v>-0.36931658188212779</v>
+        <f>'D1'!I4-'A1'!I4</f>
+        <v>0.36931658188212779</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -4600,8 +5020,8 @@
         <v>0.1</v>
       </c>
       <c r="K5">
-        <f>'A1'!I5-'D1'!I5</f>
-        <v>0.67934224243904839</v>
+        <f>'D1'!I5-'A1'!I5</f>
+        <v>-0.67934224243904839</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -4613,8 +5033,8 @@
         <v>0</v>
       </c>
       <c r="K6">
-        <f>'A1'!I6-'D1'!I6</f>
-        <v>0.6</v>
+        <f>'D1'!I6-'A1'!I6</f>
+        <v>-0.6</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -4648,8 +5068,8 @@
         <v>0.4</v>
       </c>
       <c r="K7">
-        <f>'A1'!I7-'D1'!I7</f>
-        <v>-0.2</v>
+        <f>'D1'!I7-'A1'!I7</f>
+        <v>0.2</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -4683,8 +5103,8 @@
         <v>0.2</v>
       </c>
       <c r="K8">
-        <f>'A1'!I8-'D1'!I8</f>
-        <v>-0.2</v>
+        <f>'D1'!I8-'A1'!I8</f>
+        <v>0.2</v>
       </c>
     </row>
   </sheetData>
@@ -4704,7 +5124,7 @@
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="K3" sqref="K3:K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4774,8 +5194,8 @@
         <v>53.547050852637973</v>
       </c>
       <c r="K2">
-        <f>'A1'!I2-'D2'!I2</f>
-        <v>1.8471457615275</v>
+        <f>'D2'!I2-'A1'!I2</f>
+        <v>-1.8471457615275</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -4809,8 +5229,8 @@
         <v>34.347143896069902</v>
       </c>
       <c r="K3">
-        <f>'A1'!I3-'D2'!I3</f>
-        <v>4.4778623319497299</v>
+        <f>'D2'!I3-'A1'!I3</f>
+        <v>-4.4778623319497299</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -4844,8 +5264,8 @@
         <v>12.860898654163158</v>
       </c>
       <c r="K4">
-        <f>'A1'!I4-'D2'!I4</f>
-        <v>-4.5608986541631573</v>
+        <f>'D2'!I4-'A1'!I4</f>
+        <v>4.5608986541631573</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -4879,8 +5299,8 @@
         <v>8.5732902254191217</v>
       </c>
       <c r="K5">
-        <f>'A1'!I5-'D2'!I5</f>
-        <v>-7.7939479829800735</v>
+        <f>'D2'!I5-'A1'!I5</f>
+        <v>7.7939479829800735</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -4914,8 +5334,8 @@
         <v>3.6</v>
       </c>
       <c r="K6">
-        <f>'A1'!I6-'D2'!I6</f>
-        <v>-3</v>
+        <f>'D2'!I6-'A1'!I6</f>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -4949,8 +5369,8 @@
         <v>2.5</v>
       </c>
       <c r="K7">
-        <f>'A1'!I7-'D2'!I7</f>
-        <v>-2.2999999999999998</v>
+        <f>'D2'!I7-'A1'!I7</f>
+        <v>2.2999999999999998</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -4984,8 +5404,8 @@
         <v>0.2</v>
       </c>
       <c r="K8">
-        <f>'A1'!I8-'D2'!I8</f>
-        <v>-0.2</v>
+        <f>'D2'!I8-'A1'!I8</f>
+        <v>0.2</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -5019,8 +5439,8 @@
         <v>0.8</v>
       </c>
       <c r="K9">
-        <f>'A1'!I9-'D2'!I9</f>
-        <v>-0.8</v>
+        <f>'D2'!I9-'A1'!I9</f>
+        <v>0.8</v>
       </c>
     </row>
   </sheetData>
@@ -5038,9 +5458,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
-    </sheetView>
+    <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData/>

</xml_diff>

<commit_message>
The final draft of my research paper
</commit_message>
<xml_diff>
--- a/experiments/Combined A-D.xlsx
+++ b/experiments/Combined A-D.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2220" yWindow="0" windowWidth="29480" windowHeight="19880" tabRatio="500" firstSheet="1" activeTab="9"/>
+    <workbookView xWindow="2220" yWindow="0" windowWidth="29480" windowHeight="19880" tabRatio="500" firstSheet="1" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="A1" sheetId="3" r:id="rId1"/>
@@ -350,7 +350,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -480,11 +479,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="392497720"/>
-        <c:axId val="392504616"/>
+        <c:axId val="388914520"/>
+        <c:axId val="388921416"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="392497720"/>
+        <c:axId val="388914520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -506,13 +505,12 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="392504616"/>
+        <c:crossAx val="388921416"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -520,7 +518,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="392504616"/>
+        <c:axId val="388921416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -543,21 +541,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="392497720"/>
+        <c:crossAx val="388914520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -602,7 +598,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="1"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -732,11 +727,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="392588632"/>
-        <c:axId val="392594392"/>
+        <c:axId val="389005096"/>
+        <c:axId val="408950056"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="392588632"/>
+        <c:axId val="389005096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -763,13 +758,12 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="392594392"/>
+        <c:crossAx val="408950056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -777,7 +771,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="392594392"/>
+        <c:axId val="408950056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -800,21 +794,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="392588632"/>
+        <c:crossAx val="389005096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -989,11 +981,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="392641624"/>
-        <c:axId val="392647384"/>
+        <c:axId val="408997224"/>
+        <c:axId val="409002984"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="392641624"/>
+        <c:axId val="408997224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1026,7 +1018,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="392647384"/>
+        <c:crossAx val="409002984"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1034,7 +1026,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="392647384"/>
+        <c:axId val="409002984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1069,7 +1061,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="392641624"/>
+        <c:crossAx val="408997224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1116,7 +1108,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Exercise D</a:t>
+              <a:t>Experiment D</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1254,11 +1246,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="392693944"/>
-        <c:axId val="392699464"/>
+        <c:axId val="409049480"/>
+        <c:axId val="409055000"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="392693944"/>
+        <c:axId val="409049480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1286,7 +1278,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="392699464"/>
+        <c:crossAx val="409055000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1294,7 +1286,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="392699464"/>
+        <c:axId val="409055000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1324,7 +1316,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="392693944"/>
+        <c:crossAx val="409049480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1367,10 +1359,10 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr/>
+              <a:defRPr sz="1600"/>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" sz="4000"/>
+              <a:rPr lang="en-US" sz="1600"/>
               <a:t>Distance at 0 Feet With Rotation</a:t>
             </a:r>
           </a:p>
@@ -1958,11 +1950,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="392763128"/>
-        <c:axId val="392766104"/>
+        <c:axId val="409128680"/>
+        <c:axId val="409134216"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="392763128"/>
+        <c:axId val="409128680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1975,10 +1967,10 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr sz="1000"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="2800"/>
+                  <a:rPr lang="en-US" sz="1000"/>
                   <a:t>Distance (feet)</a:t>
                 </a:r>
               </a:p>
@@ -1995,12 +1987,12 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1600"/>
+              <a:defRPr sz="1000"/>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="392766104"/>
+        <c:crossAx val="409134216"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2008,7 +2000,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="392766104"/>
+        <c:axId val="409134216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2022,10 +2014,10 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr sz="1000"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="2800"/>
+                  <a:rPr lang="en-US" sz="1000"/>
                   <a:t>Times seen per second</a:t>
                 </a:r>
               </a:p>
@@ -2043,12 +2035,12 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1600"/>
+              <a:defRPr sz="1000"/>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="392763128"/>
+        <c:crossAx val="409128680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2062,7 +2054,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1600"/>
+            <a:defRPr sz="1000"/>
           </a:pPr>
           <a:endParaRPr lang="en-US"/>
         </a:p>
@@ -2598,11 +2590,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="392812536"/>
-        <c:axId val="392815672"/>
+        <c:axId val="409189160"/>
+        <c:axId val="409194696"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="392812536"/>
+        <c:axId val="409189160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2640,7 +2632,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="392815672"/>
+        <c:crossAx val="409194696"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2648,7 +2640,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="392815672"/>
+        <c:axId val="409194696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2688,7 +2680,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="392812536"/>
+        <c:crossAx val="409189160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2829,16 +2821,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1600200</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>63500</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>901700</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>120367</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2864,16 +2856,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>317500</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>711200</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3508,7 +3500,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="S28" sqref="S28"/>
     </sheetView>
   </sheetViews>
@@ -5458,7 +5450,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData/>

</xml_diff>